<commit_message>
SEK: new 1M curve and new synthetic deposits
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK/SEK_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK/SEK_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="9600" windowHeight="12540"/>
+    <workbookView xWindow="20295" yWindow="-15" windowWidth="10200" windowHeight="8310"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -12,9 +12,9 @@
   <definedNames>
     <definedName name="Currency">MainChecks!$U$4</definedName>
     <definedName name="FirstIndex">MainChecks!$K$9</definedName>
-    <definedName name="FuturesDates">MainChecks!$C$15:$C$18</definedName>
-    <definedName name="FuturesTable">MainChecks!$A$4:$H$13</definedName>
-    <definedName name="IMMFutures">MainChecks!$D$15:$D$18</definedName>
+    <definedName name="FuturesDates">MainChecks!$C$16:$C$19</definedName>
+    <definedName name="FuturesTable">MainChecks!$A$4:$H$14</definedName>
+    <definedName name="IMMFutures">MainChecks!$D$16:$D$19</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!#REF!</definedName>
     <definedName name="TenYearsBondFutures">MainChecks!$C$4:$C$6</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
@@ -815,22 +815,22 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 16:23:45</v>
+        <v>Updated at 16:44:15</v>
         <stp/>
-        <stp>{C57868CE-1312-4D54-BB86-11DDB285789A}</stp>
-        <tr r="Q5" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 16:19:00</v>
-        <stp/>
-        <stp>{6F8A7C5C-5F70-4C69-A9D9-7D52CCF2A108}</stp>
+        <stp>{65429D61-FABF-48E8-8363-85D0EF861221}</stp>
         <tr r="Q6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 16:19:00</v>
+        <v>Updated at 16:44:15</v>
         <stp/>
-        <stp>{96895B2D-9B84-4C4F-8A00-6A2813EF7F51}</stp>
+        <stp>{1CE8C1AD-683E-4DEA-AB9B-F0AEA2E6DFCC}</stp>
         <tr r="P6" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:04:22</v>
+        <stp/>
+        <stp>{43CC7531-A0FE-4D29-A1FB-913FD1A5604E}</stp>
+        <tr r="Q5" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1222,7 +1222,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ103"/>
+  <dimension ref="A1:AJ104"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
@@ -1316,7 +1316,9 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18"/>
+      <c r="U2" s="18">
+        <v>42040.69736111111</v>
+      </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1478,14 +1480,14 @@
         <v>42069</v>
       </c>
       <c r="M5" s="26">
-        <v>154.63999999999999</v>
+        <v>158.63999999999999</v>
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 16:23:45</v>
+        <v>Updated at 17:04:22</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1546,25 +1548,25 @@
         <v>SEKAB3S10Y</v>
       </c>
       <c r="L6" s="22">
-        <v>41991</v>
+        <v>42040</v>
       </c>
       <c r="M6" s="30" t="str">
         <f>N6&amp;"/"&amp;O6</f>
-        <v>1.275/1.325</v>
+        <v>0.9825/1.0325</v>
       </c>
       <c r="N6" s="28">
-        <v>1.2749999999999999</v>
+        <v>0.98249999999999993</v>
       </c>
       <c r="O6" s="28">
-        <v>1.325</v>
+        <v>1.0325</v>
       </c>
       <c r="P6" s="28" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Updated at 16:19:00</v>
+        <v>Updated at 16:44:15</v>
       </c>
       <c r="Q6" s="29" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Updated at 16:19:00</v>
+        <v>Updated at 16:44:15</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1575,7 +1577,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>625</v>
+        <v>771</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1748,11 +1750,11 @@
       </c>
       <c r="L9" s="57">
         <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41991</v>
+        <v>42039</v>
       </c>
       <c r="M9" s="58">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>2.5800000000000003E-3</v>
+        <v>5.5999999999999995E-4</v>
       </c>
       <c r="N9" s="58"/>
       <c r="O9" s="58"/>
@@ -1814,19 +1816,19 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>SEKSTD</v>
       </c>
-      <c r="L10" s="22" t="e">
+      <c r="L10" s="22">
         <f>_xll.qlTermStructureReferenceDate(K10,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M10" s="23" t="e">
+        <v>42041</v>
+      </c>
+      <c r="M10" s="23">
         <f>_xll.qlYieldTSDiscount(K10,L10)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
       <c r="Q10" s="31" t="str">
-        <f ca="1">IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
+        <f>IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
         <v/>
       </c>
       <c r="R10" s="8" t="s">
@@ -1884,7 +1886,7 @@
       </c>
       <c r="L11" s="22">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>41995</v>
+        <v>42044</v>
       </c>
       <c r="M11" s="23">
         <f>_xll.qlYieldTSDiscount(K11,L11)</f>
@@ -1920,54 +1922,36 @@
       <c r="AJ11" s="3"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="A12" s="47"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
       <c r="K12" s="21" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>SEK3M</v>
-      </c>
-      <c r="L12" s="22" t="e">
+        <f>UPPER(Currency)&amp;"1M"</f>
+        <v>SEK1M</v>
+      </c>
+      <c r="L12" s="22">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M12" s="23" t="e">
+        <v>42044</v>
+      </c>
+      <c r="M12" s="23">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="32" t="str">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
         <v/>
       </c>
-      <c r="R12" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="R12" s="8"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -1987,44 +1971,50 @@
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
     </row>
-    <row r="13" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="53" t="s">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="53"/>
-      <c r="H13" s="54" t="s">
-        <v>36</v>
+      <c r="F13" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="39" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>SEK6M</v>
-      </c>
-      <c r="L13" s="40">
+      <c r="K13" s="21" t="str">
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>SEK3M</v>
+      </c>
+      <c r="L13" s="22">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>41995</v>
-      </c>
-      <c r="M13" s="41" t="e">
+        <v>42044</v>
+      </c>
+      <c r="M13" s="23">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="42" t="str">
-        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="32" t="str">
+        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v/>
       </c>
       <c r="R13" s="8" t="s">
@@ -2050,24 +2040,46 @@
       <c r="AJ13" s="3"/>
     </row>
     <row r="14" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="A14" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="51"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="H14" s="54" t="s">
+        <v>36</v>
+      </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="10" t="s">
+      <c r="J14" s="7"/>
+      <c r="K14" s="39" t="str">
+        <f>UPPER(Currency)&amp;"6M"</f>
+        <v>SEK6M</v>
+      </c>
+      <c r="L14" s="40">
+        <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
+        <v>42044</v>
+      </c>
+      <c r="M14" s="41">
+        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42" t="str">
+        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v/>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="S14" s="1"/>
@@ -2089,33 +2101,27 @@
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="33">
-        <f t="array" ref="C15:C18">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B15:B18)</f>
-        <v>42081</v>
-      </c>
-      <c r="D15" s="6" t="str">
-        <f t="array" ref="D15:D18">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>-H5</v>
-      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -2137,14 +2143,16 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="36" t="b">
+      <c r="B16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="34">
-        <v>42172</v>
-      </c>
-      <c r="D16" s="8" t="str">
-        <v>-M5</v>
+      <c r="C16" s="33">
+        <f t="array" ref="C16:C19">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B16:B19)</f>
+        <v>42081</v>
+      </c>
+      <c r="D16" s="6" t="str">
+        <f t="array" ref="D16:D19">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
+        <v>-H5</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2185,10 +2193,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="34">
-        <v>42263</v>
+        <v>42172</v>
       </c>
       <c r="D17" s="8" t="str">
-        <v>-U5</v>
+        <v>-M5</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2223,16 +2231,16 @@
       <c r="AI17" s="3"/>
       <c r="AJ17" s="3"/>
     </row>
-    <row r="18" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="37" t="b">
+      <c r="B18" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C18" s="35">
-        <v>42354</v>
-      </c>
-      <c r="D18" s="10" t="str">
-        <v>-Z5</v>
+      <c r="C18" s="34">
+        <v>42263</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <v>-U5</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2267,11 +2275,17 @@
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="35">
+        <v>42354</v>
+      </c>
+      <c r="D19" s="10" t="str">
+        <v>-Z5</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -3045,7 +3059,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="3"/>
+      <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
@@ -3075,14 +3089,14 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
       <c r="R40" s="3"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -3160,8 +3174,8 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
@@ -3314,19 +3328,19 @@
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="3"/>
-      <c r="AC46" s="3"/>
-      <c r="AD46" s="3"/>
-      <c r="AE46" s="3"/>
-      <c r="AF46" s="3"/>
-      <c r="AG46" s="3"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1"/>
+      <c r="AB46" s="1"/>
+      <c r="AC46" s="1"/>
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="1"/>
+      <c r="AF46" s="1"/>
+      <c r="AG46" s="1"/>
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
       <c r="AJ46" s="3"/>
@@ -5203,15 +5217,15 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="55"/>
-      <c r="K96" s="55"/>
-      <c r="L96" s="55"/>
-      <c r="M96" s="55"/>
-      <c r="N96" s="55"/>
-      <c r="O96" s="55"/>
-      <c r="P96" s="55"/>
-      <c r="Q96" s="55"/>
-      <c r="R96" s="55"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="3"/>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
+      <c r="R96" s="3"/>
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
       <c r="U96" s="3"/>
@@ -5279,15 +5293,15 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-      <c r="J98" s="43"/>
-      <c r="K98" s="43"/>
-      <c r="L98" s="43"/>
-      <c r="M98" s="43"/>
-      <c r="N98" s="43"/>
-      <c r="O98" s="43"/>
-      <c r="P98" s="43"/>
-      <c r="Q98" s="43"/>
-      <c r="R98" s="43"/>
+      <c r="J98" s="55"/>
+      <c r="K98" s="55"/>
+      <c r="L98" s="55"/>
+      <c r="M98" s="55"/>
+      <c r="N98" s="55"/>
+      <c r="O98" s="55"/>
+      <c r="P98" s="55"/>
+      <c r="Q98" s="55"/>
+      <c r="R98" s="55"/>
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
@@ -5317,6 +5331,15 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
+      <c r="J99" s="43"/>
+      <c r="K99" s="43"/>
+      <c r="L99" s="43"/>
+      <c r="M99" s="43"/>
+      <c r="N99" s="43"/>
+      <c r="O99" s="43"/>
+      <c r="P99" s="43"/>
+      <c r="Q99" s="43"/>
+      <c r="R99" s="43"/>
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
@@ -5365,7 +5388,7 @@
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
     </row>
-    <row r="101" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5374,18 +5397,35 @@
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
-      <c r="M101" s="2"/>
-      <c r="N101" s="2"/>
-      <c r="O101" s="2"/>
-      <c r="P101" s="2"/>
-      <c r="Q101" s="2"/>
-      <c r="R101" s="2"/>
-      <c r="S101" s="55"/>
+      <c r="I101" s="3"/>
+      <c r="S101" s="3"/>
+      <c r="T101" s="3"/>
+      <c r="U101" s="3"/>
+      <c r="V101" s="3"/>
+      <c r="W101" s="3"/>
+      <c r="X101" s="3"/>
+      <c r="Y101" s="3"/>
+      <c r="Z101" s="3"/>
+      <c r="AA101" s="3"/>
+      <c r="AB101" s="3"/>
+      <c r="AC101" s="3"/>
+      <c r="AD101" s="3"/>
+      <c r="AE101" s="3"/>
+      <c r="AF101" s="3"/>
+      <c r="AG101" s="3"/>
+      <c r="AH101" s="3"/>
+      <c r="AI101" s="3"/>
+      <c r="AJ101" s="3"/>
     </row>
     <row r="102" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
@@ -5397,15 +5437,27 @@
       <c r="R102" s="2"/>
       <c r="S102" s="55"/>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A103" s="43"/>
-      <c r="B103" s="43"/>
-      <c r="C103" s="43"/>
-      <c r="D103" s="43"/>
-      <c r="E103" s="43"/>
-      <c r="F103" s="43"/>
-      <c r="G103" s="43"/>
-      <c r="H103" s="43"/>
+    <row r="103" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+      <c r="M103" s="2"/>
+      <c r="N103" s="2"/>
+      <c r="O103" s="2"/>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
+      <c r="R103" s="2"/>
+      <c r="S103" s="55"/>
+    </row>
+    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A104" s="43"/>
+      <c r="B104" s="43"/>
+      <c r="C104" s="43"/>
+      <c r="D104" s="43"/>
+      <c r="E104" s="43"/>
+      <c r="F104" s="43"/>
+      <c r="G104" s="43"/>
+      <c r="H104" s="43"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5422,7 +5474,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5442,12 +5494,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5467,7 +5519,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
SEK framework with new fut/swap rate helpers
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK/SEK_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK/SEK_MainChecks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>ObjectID</t>
   </si>
@@ -815,22 +815,24 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 16:44:15</v>
+        <v>Updated at 09:28:42</v>
         <stp/>
-        <stp>{65429D61-FABF-48E8-8363-85D0EF861221}</stp>
-        <tr r="Q6" s="2"/>
+        <stp>{F884A349-5DBA-44A4-A4C8-EB715CB4E960}</stp>
+        <tr r="P6" s="2"/>
+      </tp>
+    </main>
+    <main first="pldatasource.rdatartdserver">
+      <tp t="s">
+        <v>Updated at 09:31:05</v>
+        <stp/>
+        <stp>{2EE1AE43-4443-4FFE-A2FF-0DD99F948CDF}</stp>
+        <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 16:44:15</v>
+        <v>Updated at 09:23:51</v>
         <stp/>
-        <stp>{1CE8C1AD-683E-4DEA-AB9B-F0AEA2E6DFCC}</stp>
-        <tr r="P6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 17:04:22</v>
-        <stp/>
-        <stp>{43CC7531-A0FE-4D29-A1FB-913FD1A5604E}</stp>
-        <tr r="Q5" s="2"/>
+        <stp>{AB1AAB78-A1F2-45F3-877E-167AB99F36FC}</stp>
+        <tr r="Q6" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1316,9 +1318,7 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18">
-        <v>42040.69736111111</v>
-      </c>
+      <c r="U2" s="18"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1477,17 +1477,17 @@
         <v>FGBLc1</v>
       </c>
       <c r="L5" s="25">
-        <v>42069</v>
+        <v>42163</v>
       </c>
       <c r="M5" s="26">
-        <v>158.63999999999999</v>
+        <v>153.45000000000002</v>
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 17:04:22</v>
+        <v>Updated at 09:31:05</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="U5" s="11" t="str">
         <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>1_52 / 1.5.0 / 1.5</v>
+        <v>1_57 / 1.6.0 / 1.6</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1548,25 +1548,25 @@
         <v>SEKAB3S10Y</v>
       </c>
       <c r="L6" s="22">
-        <v>42040</v>
+        <v>42137</v>
       </c>
       <c r="M6" s="30" t="str">
         <f>N6&amp;"/"&amp;O6</f>
-        <v>0.9825/1.0325</v>
+        <v>1.3525/1.4025</v>
       </c>
       <c r="N6" s="28">
-        <v>0.98249999999999993</v>
+        <v>1.3525</v>
       </c>
       <c r="O6" s="28">
-        <v>1.0325</v>
+        <v>1.4025000000000001</v>
       </c>
       <c r="P6" s="28" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Updated at 16:44:15</v>
+        <v>Updated at 09:28:42</v>
       </c>
       <c r="Q6" s="29" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Updated at 16:44:15</v>
+        <v>Updated at 09:23:51</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>771</v>
+        <v>672</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1750,11 +1750,11 @@
       </c>
       <c r="L9" s="57">
         <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>42039</v>
+        <v>42136</v>
       </c>
       <c r="M9" s="58">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>5.5999999999999995E-4</v>
+        <v>-1.9400000000000001E-3</v>
       </c>
       <c r="N9" s="58"/>
       <c r="O9" s="58"/>
@@ -1816,19 +1816,19 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>SEKSTD</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K10,Trigger)</f>
-        <v>42041</v>
-      </c>
-      <c r="M10" s="23">
+        <v>#NUM!</v>
+      </c>
+      <c r="M10" s="23" t="e">
         <f>_xll.qlYieldTSDiscount(K10,L10)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
       <c r="Q10" s="31" t="str">
-        <f>IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
+        <f ca="1">IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
         <v/>
       </c>
       <c r="R10" s="8" t="s">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="L11" s="22">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>42044</v>
+        <v>42142</v>
       </c>
       <c r="M11" s="23">
         <f>_xll.qlYieldTSDiscount(K11,L11)</f>
@@ -1936,22 +1936,24 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>SEK1M</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>42044</v>
-      </c>
-      <c r="M12" s="23">
+        <v>#NUM!</v>
+      </c>
+      <c r="M12" s="23" t="e">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="32" t="str">
-        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
         <v/>
       </c>
-      <c r="R12" s="8"/>
+      <c r="R12" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -2002,19 +2004,19 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>SEK3M</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>42044</v>
-      </c>
-      <c r="M13" s="23">
+        <v>#NUM!</v>
+      </c>
+      <c r="M13" s="23" t="e">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
       <c r="Q13" s="32" t="str">
-        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v/>
       </c>
       <c r="R13" s="8" t="s">
@@ -2064,19 +2066,19 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>SEK6M</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="40" t="e">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>42044</v>
-      </c>
-      <c r="M14" s="41">
+        <v>#NUM!</v>
+      </c>
+      <c r="M14" s="41" t="e">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="N14" s="41"/>
       <c r="O14" s="41"/>
       <c r="P14" s="41"/>
       <c r="Q14" s="42" t="str">
-        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
         <v/>
       </c>
       <c r="R14" s="8" t="s">
@@ -2148,11 +2150,11 @@
       </c>
       <c r="C16" s="33">
         <f t="array" ref="C16:C19">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B16:B19)</f>
-        <v>42081</v>
+        <v>42172</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="array" ref="D16:D19">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>-H5</v>
+        <v>-M5</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2193,10 +2195,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="34">
-        <v>42172</v>
+        <v>42263</v>
       </c>
       <c r="D17" s="8" t="str">
-        <v>-M5</v>
+        <v>-U5</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2237,10 +2239,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="34">
-        <v>42263</v>
+        <v>42354</v>
       </c>
       <c r="D18" s="8" t="str">
-        <v>-U5</v>
+        <v>-Z5</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2281,10 +2283,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="35">
-        <v>42354</v>
+        <v>42445</v>
       </c>
       <c r="D19" s="10" t="str">
-        <v>-Z5</v>
+        <v>-H6</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -5474,7 +5476,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5494,12 +5496,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5519,7 +5521,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>